<commit_message>
Updated DEU_grids model - 2025-08-31 15:02
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU_grids/Sets-vervestacks.xlsx
+++ b/VerveStacks_DEU_grids/Sets-vervestacks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr updateLinks="never" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB09D566-9DD9-4720-9D48-D9571F0A47BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{85AF9189-1BC4-4B13-A421-E49EBD04F41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4180,12 +4180,588 @@
     <t>elc*DEU_0001</t>
   </si>
   <si>
+    <t>rez_DEU_2</t>
+  </si>
+  <si>
+    <t>elc*DEU_0002</t>
+  </si>
+  <si>
+    <t>rez_DEU_3</t>
+  </si>
+  <si>
+    <t>elc*DEU_0003</t>
+  </si>
+  <si>
+    <t>rez_DEU_4</t>
+  </si>
+  <si>
+    <t>elc*DEU_0004</t>
+  </si>
+  <si>
+    <t>rez_DEU_5</t>
+  </si>
+  <si>
+    <t>elc*DEU_0005</t>
+  </si>
+  <si>
+    <t>rez_DEU_6</t>
+  </si>
+  <si>
+    <t>elc*DEU_0006</t>
+  </si>
+  <si>
+    <t>rez_DEU_7</t>
+  </si>
+  <si>
+    <t>elc*DEU_0007</t>
+  </si>
+  <si>
+    <t>rez_DEU_8</t>
+  </si>
+  <si>
+    <t>elc*DEU_0008</t>
+  </si>
+  <si>
+    <t>rez_DEU_9</t>
+  </si>
+  <si>
+    <t>elc*DEU_0009</t>
+  </si>
+  <si>
     <t>rez_DEU_10</t>
   </si>
   <si>
     <t>elc*DEU_0010</t>
   </si>
   <si>
+    <t>rez_DEU_11</t>
+  </si>
+  <si>
+    <t>elc*DEU_0011</t>
+  </si>
+  <si>
+    <t>rez_DEU_12</t>
+  </si>
+  <si>
+    <t>elc*DEU_0012</t>
+  </si>
+  <si>
+    <t>rez_DEU_13</t>
+  </si>
+  <si>
+    <t>elc*DEU_0013</t>
+  </si>
+  <si>
+    <t>rez_DEU_14</t>
+  </si>
+  <si>
+    <t>elc*DEU_0014</t>
+  </si>
+  <si>
+    <t>rez_DEU_15</t>
+  </si>
+  <si>
+    <t>elc*DEU_0015</t>
+  </si>
+  <si>
+    <t>rez_DEU_16</t>
+  </si>
+  <si>
+    <t>elc*DEU_0016</t>
+  </si>
+  <si>
+    <t>rez_DEU_17</t>
+  </si>
+  <si>
+    <t>elc*DEU_0017</t>
+  </si>
+  <si>
+    <t>rez_DEU_18</t>
+  </si>
+  <si>
+    <t>elc*DEU_0018</t>
+  </si>
+  <si>
+    <t>rez_DEU_19</t>
+  </si>
+  <si>
+    <t>elc*DEU_0019</t>
+  </si>
+  <si>
+    <t>rez_DEU_20</t>
+  </si>
+  <si>
+    <t>elc*DEU_0020</t>
+  </si>
+  <si>
+    <t>rez_DEU_21</t>
+  </si>
+  <si>
+    <t>elc*DEU_0021</t>
+  </si>
+  <si>
+    <t>rez_DEU_22</t>
+  </si>
+  <si>
+    <t>elc*DEU_0022</t>
+  </si>
+  <si>
+    <t>rez_DEU_23</t>
+  </si>
+  <si>
+    <t>elc*DEU_0023</t>
+  </si>
+  <si>
+    <t>rez_DEU_24</t>
+  </si>
+  <si>
+    <t>elc*DEU_0024</t>
+  </si>
+  <si>
+    <t>rez_DEU_25</t>
+  </si>
+  <si>
+    <t>elc*DEU_0025</t>
+  </si>
+  <si>
+    <t>rez_DEU_26</t>
+  </si>
+  <si>
+    <t>elc*DEU_0026</t>
+  </si>
+  <si>
+    <t>rez_DEU_27</t>
+  </si>
+  <si>
+    <t>elc*DEU_0027</t>
+  </si>
+  <si>
+    <t>rez_DEU_28</t>
+  </si>
+  <si>
+    <t>elc*DEU_0028</t>
+  </si>
+  <si>
+    <t>rez_DEU_29</t>
+  </si>
+  <si>
+    <t>elc*DEU_0029</t>
+  </si>
+  <si>
+    <t>rez_DEU_30</t>
+  </si>
+  <si>
+    <t>elc*DEU_0030</t>
+  </si>
+  <si>
+    <t>rez_DEU_31</t>
+  </si>
+  <si>
+    <t>elc*DEU_0031</t>
+  </si>
+  <si>
+    <t>rez_DEU_32</t>
+  </si>
+  <si>
+    <t>elc*DEU_0032</t>
+  </si>
+  <si>
+    <t>rez_DEU_33</t>
+  </si>
+  <si>
+    <t>elc*DEU_0033</t>
+  </si>
+  <si>
+    <t>rez_DEU_34</t>
+  </si>
+  <si>
+    <t>elc*DEU_0034</t>
+  </si>
+  <si>
+    <t>rez_DEU_35</t>
+  </si>
+  <si>
+    <t>elc*DEU_0035</t>
+  </si>
+  <si>
+    <t>rez_DEU_36</t>
+  </si>
+  <si>
+    <t>elc*DEU_0036</t>
+  </si>
+  <si>
+    <t>rez_DEU_37</t>
+  </si>
+  <si>
+    <t>elc*DEU_0037</t>
+  </si>
+  <si>
+    <t>rez_DEU_38</t>
+  </si>
+  <si>
+    <t>elc*DEU_0038</t>
+  </si>
+  <si>
+    <t>rez_DEU_39</t>
+  </si>
+  <si>
+    <t>elc*DEU_0039</t>
+  </si>
+  <si>
+    <t>rez_DEU_40</t>
+  </si>
+  <si>
+    <t>elc*DEU_0040</t>
+  </si>
+  <si>
+    <t>rez_DEU_41</t>
+  </si>
+  <si>
+    <t>elc*DEU_0041</t>
+  </si>
+  <si>
+    <t>rez_DEU_42</t>
+  </si>
+  <si>
+    <t>elc*DEU_0042</t>
+  </si>
+  <si>
+    <t>rez_DEU_43</t>
+  </si>
+  <si>
+    <t>elc*DEU_0043</t>
+  </si>
+  <si>
+    <t>rez_DEU_44</t>
+  </si>
+  <si>
+    <t>elc*DEU_0044</t>
+  </si>
+  <si>
+    <t>rez_DEU_45</t>
+  </si>
+  <si>
+    <t>elc*DEU_0045</t>
+  </si>
+  <si>
+    <t>rez_DEU_46</t>
+  </si>
+  <si>
+    <t>elc*DEU_0046</t>
+  </si>
+  <si>
+    <t>rez_DEU_47</t>
+  </si>
+  <si>
+    <t>elc*DEU_0047</t>
+  </si>
+  <si>
+    <t>rez_DEU_48</t>
+  </si>
+  <si>
+    <t>elc*DEU_0048</t>
+  </si>
+  <si>
+    <t>rez_DEU_49</t>
+  </si>
+  <si>
+    <t>elc*DEU_0049</t>
+  </si>
+  <si>
+    <t>rez_DEU_50</t>
+  </si>
+  <si>
+    <t>elc*DEU_0050</t>
+  </si>
+  <si>
+    <t>rez_DEU_52</t>
+  </si>
+  <si>
+    <t>elc*DEU_0052</t>
+  </si>
+  <si>
+    <t>rez_DEU_53</t>
+  </si>
+  <si>
+    <t>elc*DEU_0053</t>
+  </si>
+  <si>
+    <t>rez_DEU_54</t>
+  </si>
+  <si>
+    <t>elc*DEU_0054</t>
+  </si>
+  <si>
+    <t>rez_DEU_55</t>
+  </si>
+  <si>
+    <t>elc*DEU_0055</t>
+  </si>
+  <si>
+    <t>rez_DEU_56</t>
+  </si>
+  <si>
+    <t>elc*DEU_0056</t>
+  </si>
+  <si>
+    <t>rez_DEU_57</t>
+  </si>
+  <si>
+    <t>elc*DEU_0057</t>
+  </si>
+  <si>
+    <t>rez_DEU_58</t>
+  </si>
+  <si>
+    <t>elc*DEU_0058</t>
+  </si>
+  <si>
+    <t>rez_DEU_59</t>
+  </si>
+  <si>
+    <t>elc*DEU_0059</t>
+  </si>
+  <si>
+    <t>rez_DEU_60</t>
+  </si>
+  <si>
+    <t>elc*DEU_0060</t>
+  </si>
+  <si>
+    <t>rez_DEU_61</t>
+  </si>
+  <si>
+    <t>elc*DEU_0061</t>
+  </si>
+  <si>
+    <t>rez_DEU_62</t>
+  </si>
+  <si>
+    <t>elc*DEU_0062</t>
+  </si>
+  <si>
+    <t>rez_DEU_63</t>
+  </si>
+  <si>
+    <t>elc*DEU_0063</t>
+  </si>
+  <si>
+    <t>rez_DEU_64</t>
+  </si>
+  <si>
+    <t>elc*DEU_0064</t>
+  </si>
+  <si>
+    <t>rez_DEU_65</t>
+  </si>
+  <si>
+    <t>elc*DEU_0065</t>
+  </si>
+  <si>
+    <t>rez_DEU_66</t>
+  </si>
+  <si>
+    <t>elc*DEU_0066</t>
+  </si>
+  <si>
+    <t>rez_DEU_67</t>
+  </si>
+  <si>
+    <t>elc*DEU_0067</t>
+  </si>
+  <si>
+    <t>rez_DEU_68</t>
+  </si>
+  <si>
+    <t>elc*DEU_0068</t>
+  </si>
+  <si>
+    <t>rez_DEU_69</t>
+  </si>
+  <si>
+    <t>elc*DEU_0069</t>
+  </si>
+  <si>
+    <t>rez_DEU_70</t>
+  </si>
+  <si>
+    <t>elc*DEU_0070</t>
+  </si>
+  <si>
+    <t>rez_DEU_71</t>
+  </si>
+  <si>
+    <t>elc*DEU_0071</t>
+  </si>
+  <si>
+    <t>rez_DEU_72</t>
+  </si>
+  <si>
+    <t>elc*DEU_0072</t>
+  </si>
+  <si>
+    <t>rez_DEU_73</t>
+  </si>
+  <si>
+    <t>elc*DEU_0073</t>
+  </si>
+  <si>
+    <t>rez_DEU_74</t>
+  </si>
+  <si>
+    <t>elc*DEU_0074</t>
+  </si>
+  <si>
+    <t>rez_DEU_75</t>
+  </si>
+  <si>
+    <t>elc*DEU_0075</t>
+  </si>
+  <si>
+    <t>rez_DEU_76</t>
+  </si>
+  <si>
+    <t>elc*DEU_0076</t>
+  </si>
+  <si>
+    <t>rez_DEU_77</t>
+  </si>
+  <si>
+    <t>elc*DEU_0077</t>
+  </si>
+  <si>
+    <t>rez_DEU_78</t>
+  </si>
+  <si>
+    <t>elc*DEU_0078</t>
+  </si>
+  <si>
+    <t>rez_DEU_79</t>
+  </si>
+  <si>
+    <t>elc*DEU_0079</t>
+  </si>
+  <si>
+    <t>rez_DEU_80</t>
+  </si>
+  <si>
+    <t>elc*DEU_0080</t>
+  </si>
+  <si>
+    <t>rez_DEU_81</t>
+  </si>
+  <si>
+    <t>elc*DEU_0081</t>
+  </si>
+  <si>
+    <t>rez_DEU_82</t>
+  </si>
+  <si>
+    <t>elc*DEU_0082</t>
+  </si>
+  <si>
+    <t>rez_DEU_83</t>
+  </si>
+  <si>
+    <t>elc*DEU_0083</t>
+  </si>
+  <si>
+    <t>rez_DEU_84</t>
+  </si>
+  <si>
+    <t>elc*DEU_0084</t>
+  </si>
+  <si>
+    <t>rez_DEU_85</t>
+  </si>
+  <si>
+    <t>elc*DEU_0085</t>
+  </si>
+  <si>
+    <t>rez_DEU_86</t>
+  </si>
+  <si>
+    <t>elc*DEU_0086</t>
+  </si>
+  <si>
+    <t>rez_DEU_87</t>
+  </si>
+  <si>
+    <t>elc*DEU_0087</t>
+  </si>
+  <si>
+    <t>rez_DEU_88</t>
+  </si>
+  <si>
+    <t>elc*DEU_0088</t>
+  </si>
+  <si>
+    <t>rez_DEU_89</t>
+  </si>
+  <si>
+    <t>elc*DEU_0089</t>
+  </si>
+  <si>
+    <t>rez_DEU_90</t>
+  </si>
+  <si>
+    <t>elc*DEU_0090</t>
+  </si>
+  <si>
+    <t>rez_DEU_91</t>
+  </si>
+  <si>
+    <t>elc*DEU_0091</t>
+  </si>
+  <si>
+    <t>rez_DEU_92</t>
+  </si>
+  <si>
+    <t>elc*DEU_0092</t>
+  </si>
+  <si>
+    <t>rez_DEU_93</t>
+  </si>
+  <si>
+    <t>elc*DEU_0093</t>
+  </si>
+  <si>
+    <t>rez_DEU_94</t>
+  </si>
+  <si>
+    <t>elc*DEU_0094</t>
+  </si>
+  <si>
+    <t>rez_DEU_95</t>
+  </si>
+  <si>
+    <t>elc*DEU_0095</t>
+  </si>
+  <si>
+    <t>rez_DEU_96</t>
+  </si>
+  <si>
+    <t>elc*DEU_0096</t>
+  </si>
+  <si>
+    <t>rez_DEU_97</t>
+  </si>
+  <si>
+    <t>elc*DEU_0097</t>
+  </si>
+  <si>
+    <t>rez_DEU_98</t>
+  </si>
+  <si>
+    <t>elc*DEU_0098</t>
+  </si>
+  <si>
+    <t>rez_DEU_99</t>
+  </si>
+  <si>
+    <t>elc*DEU_0099</t>
+  </si>
+  <si>
     <t>rez_DEU_100</t>
   </si>
   <si>
@@ -4246,12 +4822,6 @@
     <t>elc*DEU_0109</t>
   </si>
   <si>
-    <t>rez_DEU_11</t>
-  </si>
-  <si>
-    <t>elc*DEU_0011</t>
-  </si>
-  <si>
     <t>rez_DEU_110</t>
   </si>
   <si>
@@ -4312,12 +4882,6 @@
     <t>elc*DEU_0119</t>
   </si>
   <si>
-    <t>rez_DEU_12</t>
-  </si>
-  <si>
-    <t>elc*DEU_0012</t>
-  </si>
-  <si>
     <t>rez_DEU_120</t>
   </si>
   <si>
@@ -4378,12 +4942,6 @@
     <t>elc*DEU_0129</t>
   </si>
   <si>
-    <t>rez_DEU_13</t>
-  </si>
-  <si>
-    <t>elc*DEU_0013</t>
-  </si>
-  <si>
     <t>rez_DEU_130</t>
   </si>
   <si>
@@ -4444,12 +5002,6 @@
     <t>elc*DEU_0139</t>
   </si>
   <si>
-    <t>rez_DEU_14</t>
-  </si>
-  <si>
-    <t>elc*DEU_0014</t>
-  </si>
-  <si>
     <t>rez_DEU_140</t>
   </si>
   <si>
@@ -4510,12 +5062,6 @@
     <t>elc*DEU_0149</t>
   </si>
   <si>
-    <t>rez_DEU_15</t>
-  </si>
-  <si>
-    <t>elc*DEU_0015</t>
-  </si>
-  <si>
     <t>rez_DEU_150</t>
   </si>
   <si>
@@ -4576,12 +5122,6 @@
     <t>elc*DEU_0159</t>
   </si>
   <si>
-    <t>rez_DEU_16</t>
-  </si>
-  <si>
-    <t>elc*DEU_0016</t>
-  </si>
-  <si>
     <t>rez_DEU_160</t>
   </si>
   <si>
@@ -4642,12 +5182,6 @@
     <t>elc*DEU_0169</t>
   </si>
   <si>
-    <t>rez_DEU_17</t>
-  </si>
-  <si>
-    <t>elc*DEU_0017</t>
-  </si>
-  <si>
     <t>rez_DEU_170</t>
   </si>
   <si>
@@ -4708,12 +5242,6 @@
     <t>elc*DEU_0179</t>
   </si>
   <si>
-    <t>rez_DEU_18</t>
-  </si>
-  <si>
-    <t>elc*DEU_0018</t>
-  </si>
-  <si>
     <t>rez_DEU_180</t>
   </si>
   <si>
@@ -4766,534 +5294,6 @@
   </si>
   <si>
     <t>elc*DEU_0188</t>
-  </si>
-  <si>
-    <t>rez_DEU_19</t>
-  </si>
-  <si>
-    <t>elc*DEU_0019</t>
-  </si>
-  <si>
-    <t>rez_DEU_2</t>
-  </si>
-  <si>
-    <t>elc*DEU_0002</t>
-  </si>
-  <si>
-    <t>rez_DEU_20</t>
-  </si>
-  <si>
-    <t>elc*DEU_0020</t>
-  </si>
-  <si>
-    <t>rez_DEU_21</t>
-  </si>
-  <si>
-    <t>elc*DEU_0021</t>
-  </si>
-  <si>
-    <t>rez_DEU_22</t>
-  </si>
-  <si>
-    <t>elc*DEU_0022</t>
-  </si>
-  <si>
-    <t>rez_DEU_23</t>
-  </si>
-  <si>
-    <t>elc*DEU_0023</t>
-  </si>
-  <si>
-    <t>rez_DEU_24</t>
-  </si>
-  <si>
-    <t>elc*DEU_0024</t>
-  </si>
-  <si>
-    <t>rez_DEU_25</t>
-  </si>
-  <si>
-    <t>elc*DEU_0025</t>
-  </si>
-  <si>
-    <t>rez_DEU_26</t>
-  </si>
-  <si>
-    <t>elc*DEU_0026</t>
-  </si>
-  <si>
-    <t>rez_DEU_27</t>
-  </si>
-  <si>
-    <t>elc*DEU_0027</t>
-  </si>
-  <si>
-    <t>rez_DEU_28</t>
-  </si>
-  <si>
-    <t>elc*DEU_0028</t>
-  </si>
-  <si>
-    <t>rez_DEU_29</t>
-  </si>
-  <si>
-    <t>elc*DEU_0029</t>
-  </si>
-  <si>
-    <t>rez_DEU_3</t>
-  </si>
-  <si>
-    <t>elc*DEU_0003</t>
-  </si>
-  <si>
-    <t>rez_DEU_30</t>
-  </si>
-  <si>
-    <t>elc*DEU_0030</t>
-  </si>
-  <si>
-    <t>rez_DEU_31</t>
-  </si>
-  <si>
-    <t>elc*DEU_0031</t>
-  </si>
-  <si>
-    <t>rez_DEU_32</t>
-  </si>
-  <si>
-    <t>elc*DEU_0032</t>
-  </si>
-  <si>
-    <t>rez_DEU_33</t>
-  </si>
-  <si>
-    <t>elc*DEU_0033</t>
-  </si>
-  <si>
-    <t>rez_DEU_34</t>
-  </si>
-  <si>
-    <t>elc*DEU_0034</t>
-  </si>
-  <si>
-    <t>rez_DEU_35</t>
-  </si>
-  <si>
-    <t>elc*DEU_0035</t>
-  </si>
-  <si>
-    <t>rez_DEU_36</t>
-  </si>
-  <si>
-    <t>elc*DEU_0036</t>
-  </si>
-  <si>
-    <t>rez_DEU_37</t>
-  </si>
-  <si>
-    <t>elc*DEU_0037</t>
-  </si>
-  <si>
-    <t>rez_DEU_38</t>
-  </si>
-  <si>
-    <t>elc*DEU_0038</t>
-  </si>
-  <si>
-    <t>rez_DEU_39</t>
-  </si>
-  <si>
-    <t>elc*DEU_0039</t>
-  </si>
-  <si>
-    <t>rez_DEU_4</t>
-  </si>
-  <si>
-    <t>elc*DEU_0004</t>
-  </si>
-  <si>
-    <t>rez_DEU_40</t>
-  </si>
-  <si>
-    <t>elc*DEU_0040</t>
-  </si>
-  <si>
-    <t>rez_DEU_41</t>
-  </si>
-  <si>
-    <t>elc*DEU_0041</t>
-  </si>
-  <si>
-    <t>rez_DEU_42</t>
-  </si>
-  <si>
-    <t>elc*DEU_0042</t>
-  </si>
-  <si>
-    <t>rez_DEU_43</t>
-  </si>
-  <si>
-    <t>elc*DEU_0043</t>
-  </si>
-  <si>
-    <t>rez_DEU_44</t>
-  </si>
-  <si>
-    <t>elc*DEU_0044</t>
-  </si>
-  <si>
-    <t>rez_DEU_45</t>
-  </si>
-  <si>
-    <t>elc*DEU_0045</t>
-  </si>
-  <si>
-    <t>rez_DEU_46</t>
-  </si>
-  <si>
-    <t>elc*DEU_0046</t>
-  </si>
-  <si>
-    <t>rez_DEU_47</t>
-  </si>
-  <si>
-    <t>elc*DEU_0047</t>
-  </si>
-  <si>
-    <t>rez_DEU_48</t>
-  </si>
-  <si>
-    <t>elc*DEU_0048</t>
-  </si>
-  <si>
-    <t>rez_DEU_49</t>
-  </si>
-  <si>
-    <t>elc*DEU_0049</t>
-  </si>
-  <si>
-    <t>rez_DEU_5</t>
-  </si>
-  <si>
-    <t>elc*DEU_0005</t>
-  </si>
-  <si>
-    <t>rez_DEU_50</t>
-  </si>
-  <si>
-    <t>elc*DEU_0050</t>
-  </si>
-  <si>
-    <t>rez_DEU_52</t>
-  </si>
-  <si>
-    <t>elc*DEU_0052</t>
-  </si>
-  <si>
-    <t>rez_DEU_53</t>
-  </si>
-  <si>
-    <t>elc*DEU_0053</t>
-  </si>
-  <si>
-    <t>rez_DEU_54</t>
-  </si>
-  <si>
-    <t>elc*DEU_0054</t>
-  </si>
-  <si>
-    <t>rez_DEU_55</t>
-  </si>
-  <si>
-    <t>elc*DEU_0055</t>
-  </si>
-  <si>
-    <t>rez_DEU_56</t>
-  </si>
-  <si>
-    <t>elc*DEU_0056</t>
-  </si>
-  <si>
-    <t>rez_DEU_57</t>
-  </si>
-  <si>
-    <t>elc*DEU_0057</t>
-  </si>
-  <si>
-    <t>rez_DEU_58</t>
-  </si>
-  <si>
-    <t>elc*DEU_0058</t>
-  </si>
-  <si>
-    <t>rez_DEU_59</t>
-  </si>
-  <si>
-    <t>elc*DEU_0059</t>
-  </si>
-  <si>
-    <t>rez_DEU_6</t>
-  </si>
-  <si>
-    <t>elc*DEU_0006</t>
-  </si>
-  <si>
-    <t>rez_DEU_60</t>
-  </si>
-  <si>
-    <t>elc*DEU_0060</t>
-  </si>
-  <si>
-    <t>rez_DEU_61</t>
-  </si>
-  <si>
-    <t>elc*DEU_0061</t>
-  </si>
-  <si>
-    <t>rez_DEU_62</t>
-  </si>
-  <si>
-    <t>elc*DEU_0062</t>
-  </si>
-  <si>
-    <t>rez_DEU_63</t>
-  </si>
-  <si>
-    <t>elc*DEU_0063</t>
-  </si>
-  <si>
-    <t>rez_DEU_64</t>
-  </si>
-  <si>
-    <t>elc*DEU_0064</t>
-  </si>
-  <si>
-    <t>rez_DEU_65</t>
-  </si>
-  <si>
-    <t>elc*DEU_0065</t>
-  </si>
-  <si>
-    <t>rez_DEU_66</t>
-  </si>
-  <si>
-    <t>elc*DEU_0066</t>
-  </si>
-  <si>
-    <t>rez_DEU_67</t>
-  </si>
-  <si>
-    <t>elc*DEU_0067</t>
-  </si>
-  <si>
-    <t>rez_DEU_68</t>
-  </si>
-  <si>
-    <t>elc*DEU_0068</t>
-  </si>
-  <si>
-    <t>rez_DEU_69</t>
-  </si>
-  <si>
-    <t>elc*DEU_0069</t>
-  </si>
-  <si>
-    <t>rez_DEU_7</t>
-  </si>
-  <si>
-    <t>elc*DEU_0007</t>
-  </si>
-  <si>
-    <t>rez_DEU_70</t>
-  </si>
-  <si>
-    <t>elc*DEU_0070</t>
-  </si>
-  <si>
-    <t>rez_DEU_71</t>
-  </si>
-  <si>
-    <t>elc*DEU_0071</t>
-  </si>
-  <si>
-    <t>rez_DEU_72</t>
-  </si>
-  <si>
-    <t>elc*DEU_0072</t>
-  </si>
-  <si>
-    <t>rez_DEU_73</t>
-  </si>
-  <si>
-    <t>elc*DEU_0073</t>
-  </si>
-  <si>
-    <t>rez_DEU_74</t>
-  </si>
-  <si>
-    <t>elc*DEU_0074</t>
-  </si>
-  <si>
-    <t>rez_DEU_75</t>
-  </si>
-  <si>
-    <t>elc*DEU_0075</t>
-  </si>
-  <si>
-    <t>rez_DEU_76</t>
-  </si>
-  <si>
-    <t>elc*DEU_0076</t>
-  </si>
-  <si>
-    <t>rez_DEU_77</t>
-  </si>
-  <si>
-    <t>elc*DEU_0077</t>
-  </si>
-  <si>
-    <t>rez_DEU_78</t>
-  </si>
-  <si>
-    <t>elc*DEU_0078</t>
-  </si>
-  <si>
-    <t>rez_DEU_79</t>
-  </si>
-  <si>
-    <t>elc*DEU_0079</t>
-  </si>
-  <si>
-    <t>rez_DEU_8</t>
-  </si>
-  <si>
-    <t>elc*DEU_0008</t>
-  </si>
-  <si>
-    <t>rez_DEU_80</t>
-  </si>
-  <si>
-    <t>elc*DEU_0080</t>
-  </si>
-  <si>
-    <t>rez_DEU_81</t>
-  </si>
-  <si>
-    <t>elc*DEU_0081</t>
-  </si>
-  <si>
-    <t>rez_DEU_82</t>
-  </si>
-  <si>
-    <t>elc*DEU_0082</t>
-  </si>
-  <si>
-    <t>rez_DEU_83</t>
-  </si>
-  <si>
-    <t>elc*DEU_0083</t>
-  </si>
-  <si>
-    <t>rez_DEU_84</t>
-  </si>
-  <si>
-    <t>elc*DEU_0084</t>
-  </si>
-  <si>
-    <t>rez_DEU_85</t>
-  </si>
-  <si>
-    <t>elc*DEU_0085</t>
-  </si>
-  <si>
-    <t>rez_DEU_86</t>
-  </si>
-  <si>
-    <t>elc*DEU_0086</t>
-  </si>
-  <si>
-    <t>rez_DEU_87</t>
-  </si>
-  <si>
-    <t>elc*DEU_0087</t>
-  </si>
-  <si>
-    <t>rez_DEU_88</t>
-  </si>
-  <si>
-    <t>elc*DEU_0088</t>
-  </si>
-  <si>
-    <t>rez_DEU_89</t>
-  </si>
-  <si>
-    <t>elc*DEU_0089</t>
-  </si>
-  <si>
-    <t>rez_DEU_9</t>
-  </si>
-  <si>
-    <t>elc*DEU_0009</t>
-  </si>
-  <si>
-    <t>rez_DEU_90</t>
-  </si>
-  <si>
-    <t>elc*DEU_0090</t>
-  </si>
-  <si>
-    <t>rez_DEU_91</t>
-  </si>
-  <si>
-    <t>elc*DEU_0091</t>
-  </si>
-  <si>
-    <t>rez_DEU_92</t>
-  </si>
-  <si>
-    <t>elc*DEU_0092</t>
-  </si>
-  <si>
-    <t>rez_DEU_93</t>
-  </si>
-  <si>
-    <t>elc*DEU_0093</t>
-  </si>
-  <si>
-    <t>rez_DEU_94</t>
-  </si>
-  <si>
-    <t>elc*DEU_0094</t>
-  </si>
-  <si>
-    <t>rez_DEU_95</t>
-  </si>
-  <si>
-    <t>elc*DEU_0095</t>
-  </si>
-  <si>
-    <t>rez_DEU_96</t>
-  </si>
-  <si>
-    <t>elc*DEU_0096</t>
-  </si>
-  <si>
-    <t>rez_DEU_97</t>
-  </si>
-  <si>
-    <t>elc*DEU_0097</t>
-  </si>
-  <si>
-    <t>rez_DEU_98</t>
-  </si>
-  <si>
-    <t>elc*DEU_0098</t>
-  </si>
-  <si>
-    <t>rez_DEU_99</t>
-  </si>
-  <si>
-    <t>elc*DEU_0099</t>
   </si>
   <si>
     <t>VERVESTACKS - the open USE platform · Powered by data · Shaped by vision · Guided by intuition · Fueled by passion</t>
@@ -5494,7 +5494,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D056FD3-1304-8747-84EC-696771C82128}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D1B3D49-C91D-7A01-7C51-416489E6FE7B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6276,7 +6276,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41FD01B-BC74-4E32-A91F-4EE6802853CB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7572081E-A565-42DD-8D8C-0EED759F4859}">
   <dimension ref="A1:H829"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated DEU_grids model - 2025-09-06 14:42
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU_grids/Sets-vervestacks.xlsx
+++ b/VerveStacks_DEU_grids/Sets-vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{740F056E-275D-47F1-994F-062FB6CD7058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{28B4B954-79B2-4906-9B67-6AFBA087C28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6367,7 +6367,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E96A572-6CDA-4114-804A-7AD5E73692EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EAD47CD-5BC5-4117-9BA7-E67290F49ACE}">
   <dimension ref="B2:C867"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated DEU_grids model - 2025-09-06 14:48
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU_grids/Sets-vervestacks.xlsx
+++ b/VerveStacks_DEU_grids/Sets-vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28B4B954-79B2-4906-9B67-6AFBA087C28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC9DCDF5-1391-4056-A0AF-F532E7F93202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6367,7 +6367,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EAD47CD-5BC5-4117-9BA7-E67290F49ACE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA7C4DA-A3AF-4207-9894-41FEECEB6AF8}">
   <dimension ref="B2:C867"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>